<commit_message>
"Updated History page with DateRangePicker styling, removed global Rsuite CSS import, and made changes to Historique.module.css, globals.css, and sidebar.module.css files."
</commit_message>
<xml_diff>
--- a/public/subscriptions.xlsx
+++ b/public/subscriptions.xlsx
@@ -469,7 +469,7 @@
         <v>PayAsYouGo_2014-09-01</v>
       </c>
       <c r="G3" s="1">
-        <v>45605.73618</v>
+        <v>45631.34992359954</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         <v>MSDN_2014-09-01</v>
       </c>
       <c r="G4" s="1">
-        <v>45605.73618133102</v>
+        <v>45631.349926828705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>